<commit_message>
Update supp-info with gpt-4o data; update citation; rm .Rhistory
</commit_message>
<xml_diff>
--- a/data/Supplementary Tables.xlsx
+++ b/data/Supplementary Tables.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ziyi Ding\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ziyi Ding\Desktop\BRM drafts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F046AD97-54D7-4516-8168-644391CC4CEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB3C7104-44C1-4730-A347-6FC177A49A95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14925" yWindow="570" windowWidth="13875" windowHeight="14460" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Supplementary Table 1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="731" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="691" uniqueCount="49">
   <si>
     <t>Variables</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -140,34 +140,6 @@
   </si>
   <si>
     <t>&lt; .001</t>
-  </si>
-  <si>
-    <t>4756</t>
-  </si>
-  <si>
-    <t>4756</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>2274</t>
-  </si>
-  <si>
-    <t>2274</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>601</t>
-  </si>
-  <si>
-    <t>601</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>347</t>
-  </si>
-  <si>
-    <t>347</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>SWOW-ZH R1 strength</t>
@@ -291,34 +263,73 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Supplementary Table 1 Partial Correlations between Lexical Decision Tasks and Word Accessibility Measurements</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Supplementary Table 2 Correlation Coefficients for Relatedness judgment Tasks and Semantic Similarity Tasks</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Supplementary Table 3 Correlation Coefficients for Relatedness Judgment Tasks and Random Walk Estimates in Different Numbers of Participants</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Relatedness Ratings (Abstract)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>GPT-3.5-turbo R1 RW</t>
-  </si>
-  <si>
-    <t>GPT-3.5-turbo R1 RW</t>
+    <r>
+      <t xml:space="preserve">Supplementary Table 1 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF374151"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t>Partial Correlations between Lexical Decision Tasks and Word Accessibility Measurements</t>
+    </r>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>GPT-3.5-turbo R123 RW</t>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FF374151"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t>Supplementary Table 2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF374151"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> Correlation Coefficients for Relatedness judgment Tasks and Semantic Similarity Tasks</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>GPT-3.5-turbo R123 RW</t>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FF374151"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t>Supplementary Table 3</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF374151"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> Correlation Coefficients for Relatedness Judgment Tasks and Random Walk Estimates in Different Numbers of Participants</t>
+    </r>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>GPT-4o R1 RW</t>
+  </si>
+  <si>
+    <t>GPT-4o R123 RW</t>
   </si>
 </sst>
 </file>
@@ -331,7 +342,7 @@
     <numFmt numFmtId="178" formatCode="0_ "/>
     <numFmt numFmtId="179" formatCode="0.000"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -372,6 +383,13 @@
       <name val="Segoe UI"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF374151"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -381,7 +399,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -389,11 +407,31 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -405,6 +443,15 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="177" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="178" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -685,19 +732,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:H42"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="34.625" style="8" customWidth="1"/>
+    <col min="1" max="1" width="10.75" customWidth="1"/>
+    <col min="2" max="2" width="20.25" style="8" customWidth="1"/>
     <col min="3" max="3" width="54.125" style="8" customWidth="1"/>
+    <col min="4" max="4" width="7.25" customWidth="1"/>
+    <col min="5" max="5" width="20" customWidth="1"/>
+    <col min="6" max="6" width="14.25" customWidth="1"/>
+    <col min="7" max="7" width="14" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>51</v>
+      <c r="A1" s="11" t="s">
+        <v>44</v>
       </c>
       <c r="B1" s="7"/>
       <c r="C1" s="7"/>
@@ -708,28 +765,28 @@
       <c r="H1" s="2"/>
     </row>
     <row r="2" spans="1:8" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F2" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="G2" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="H2" s="12" t="s">
         <v>1</v>
       </c>
     </row>
@@ -743,8 +800,8 @@
       <c r="C3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>28</v>
+      <c r="D3" s="18">
+        <v>4756</v>
       </c>
       <c r="E3" s="3">
         <v>-0.51600000000000001</v>
@@ -769,8 +826,8 @@
       <c r="C4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="1" t="s">
-        <v>28</v>
+      <c r="D4" s="18">
+        <v>4756</v>
       </c>
       <c r="E4" s="3">
         <v>-0.52</v>
@@ -790,13 +847,13 @@
         <v>10</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="1" t="s">
-        <v>27</v>
+      <c r="D5" s="18">
+        <v>4756</v>
       </c>
       <c r="E5" s="3">
         <v>-0.52600000000000002</v>
@@ -816,13 +873,13 @@
         <v>10</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D6" s="1" t="s">
-        <v>27</v>
+      <c r="D6" s="18">
+        <v>4756</v>
       </c>
       <c r="E6" s="3">
         <v>-0.46800000000000003</v>
@@ -842,13 +899,13 @@
         <v>10</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D7" s="1" t="s">
-        <v>27</v>
+      <c r="D7" s="18">
+        <v>4756</v>
       </c>
       <c r="E7" s="3">
         <v>-0.47499999999999998</v>
@@ -871,10 +928,10 @@
         <v>8</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>27</v>
+        <v>38</v>
+      </c>
+      <c r="D8" s="18">
+        <v>4756</v>
       </c>
       <c r="E8" s="3">
         <v>-0.378</v>
@@ -897,10 +954,10 @@
         <v>9</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>27</v>
+        <v>38</v>
+      </c>
+      <c r="D9" s="18">
+        <v>4756</v>
       </c>
       <c r="E9" s="3">
         <v>-0.38300000000000001</v>
@@ -920,13 +977,13 @@
         <v>10</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>27</v>
+        <v>38</v>
+      </c>
+      <c r="D10" s="18">
+        <v>4756</v>
       </c>
       <c r="E10" s="3">
         <v>-0.39</v>
@@ -946,13 +1003,13 @@
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>27</v>
+        <v>34</v>
+      </c>
+      <c r="D11" s="18">
+        <v>4756</v>
       </c>
       <c r="E11" s="3">
         <v>-0.246</v>
@@ -972,13 +1029,13 @@
         <v>10</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>27</v>
+        <v>34</v>
+      </c>
+      <c r="D12" s="18">
+        <v>4756</v>
       </c>
       <c r="E12" s="3">
         <v>-0.255</v>
@@ -1003,8 +1060,8 @@
       <c r="C13" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D13" s="1" t="s">
-        <v>30</v>
+      <c r="D13" s="18">
+        <v>4756</v>
       </c>
       <c r="E13" s="3">
         <v>-0.51100000000000001</v>
@@ -1029,8 +1086,8 @@
       <c r="C14" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D14" s="1" t="s">
-        <v>30</v>
+      <c r="D14" s="18">
+        <v>4756</v>
       </c>
       <c r="E14" s="3">
         <v>-0.49299999999999999</v>
@@ -1050,13 +1107,13 @@
         <v>13</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D15" s="1" t="s">
-        <v>29</v>
+      <c r="D15" s="18">
+        <v>4756</v>
       </c>
       <c r="E15" s="3">
         <v>-0.501</v>
@@ -1076,13 +1133,13 @@
         <v>13</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D16" s="1" t="s">
-        <v>29</v>
+      <c r="D16" s="18">
+        <v>4756</v>
       </c>
       <c r="E16" s="3">
         <v>-0.51600000000000001</v>
@@ -1102,13 +1159,13 @@
         <v>13</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D17" s="1" t="s">
-        <v>29</v>
+      <c r="D17" s="18">
+        <v>4756</v>
       </c>
       <c r="E17" s="3">
         <v>-0.52900000000000003</v>
@@ -1131,10 +1188,10 @@
         <v>8</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>29</v>
+        <v>38</v>
+      </c>
+      <c r="D18" s="18">
+        <v>4756</v>
       </c>
       <c r="E18" s="3">
         <v>-0.3</v>
@@ -1157,10 +1214,10 @@
         <v>9</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>29</v>
+        <v>38</v>
+      </c>
+      <c r="D19" s="18">
+        <v>4756</v>
       </c>
       <c r="E19" s="3">
         <v>-0.27500000000000002</v>
@@ -1180,13 +1237,13 @@
         <v>13</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>29</v>
+        <v>38</v>
+      </c>
+      <c r="D20" s="18">
+        <v>4756</v>
       </c>
       <c r="E20" s="3">
         <v>-0.28100000000000003</v>
@@ -1206,13 +1263,13 @@
         <v>13</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>29</v>
+        <v>34</v>
+      </c>
+      <c r="D21" s="18">
+        <v>4756</v>
       </c>
       <c r="E21" s="3">
         <v>-0.249</v>
@@ -1232,13 +1289,13 @@
         <v>13</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>29</v>
+        <v>34</v>
+      </c>
+      <c r="D22" s="18">
+        <v>4756</v>
       </c>
       <c r="E22" s="3">
         <v>-0.25900000000000001</v>
@@ -1263,8 +1320,8 @@
       <c r="C23" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D23" s="1" t="s">
-        <v>32</v>
+      <c r="D23" s="18">
+        <v>4756</v>
       </c>
       <c r="E23" s="3">
         <v>-0.52100000000000002</v>
@@ -1289,8 +1346,8 @@
       <c r="C24" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D24" s="1" t="s">
-        <v>32</v>
+      <c r="D24" s="18">
+        <v>4756</v>
       </c>
       <c r="E24" s="3">
         <v>-0.53400000000000003</v>
@@ -1310,13 +1367,13 @@
         <v>14</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D25" s="1" t="s">
-        <v>31</v>
+      <c r="D25" s="18">
+        <v>4756</v>
       </c>
       <c r="E25" s="3">
         <v>-0.53800000000000003</v>
@@ -1336,13 +1393,13 @@
         <v>14</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D26" s="1" t="s">
-        <v>31</v>
+      <c r="D26" s="18">
+        <v>4756</v>
       </c>
       <c r="E26" s="3">
         <v>-0.41699999999999998</v>
@@ -1362,13 +1419,13 @@
         <v>14</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D27" s="1" t="s">
-        <v>31</v>
+      <c r="D27" s="18">
+        <v>4756</v>
       </c>
       <c r="E27" s="3">
         <v>-0.43099999999999999</v>
@@ -1391,10 +1448,10 @@
         <v>8</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="D28" s="1" t="s">
-        <v>31</v>
+        <v>38</v>
+      </c>
+      <c r="D28" s="18">
+        <v>4756</v>
       </c>
       <c r="E28" s="3">
         <v>-0.437</v>
@@ -1417,10 +1474,10 @@
         <v>9</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="D29" s="1" t="s">
-        <v>31</v>
+        <v>38</v>
+      </c>
+      <c r="D29" s="18">
+        <v>4756</v>
       </c>
       <c r="E29" s="3">
         <v>-0.42899999999999999</v>
@@ -1440,13 +1497,13 @@
         <v>14</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="D30" s="1" t="s">
-        <v>31</v>
+        <v>38</v>
+      </c>
+      <c r="D30" s="18">
+        <v>4756</v>
       </c>
       <c r="E30" s="3">
         <v>-0.437</v>
@@ -1466,13 +1523,13 @@
         <v>14</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D31" s="1" t="s">
-        <v>31</v>
+        <v>34</v>
+      </c>
+      <c r="D31" s="18">
+        <v>4756</v>
       </c>
       <c r="E31" s="3">
         <v>-0.23499999999999999</v>
@@ -1492,13 +1549,13 @@
         <v>14</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D32" s="1" t="s">
-        <v>31</v>
+        <v>34</v>
+      </c>
+      <c r="D32" s="18">
+        <v>4756</v>
       </c>
       <c r="E32" s="3">
         <v>-0.25900000000000001</v>
@@ -1523,8 +1580,8 @@
       <c r="C33" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D33" s="1" t="s">
-        <v>34</v>
+      <c r="D33" s="18">
+        <v>4756</v>
       </c>
       <c r="E33" s="3">
         <v>-0.56799999999999995</v>
@@ -1549,8 +1606,8 @@
       <c r="C34" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D34" s="1" t="s">
-        <v>34</v>
+      <c r="D34" s="18">
+        <v>4756</v>
       </c>
       <c r="E34" s="3">
         <v>-0.61899999999999999</v>
@@ -1570,13 +1627,13 @@
         <v>15</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D35" s="1" t="s">
-        <v>33</v>
+      <c r="D35" s="18">
+        <v>4756</v>
       </c>
       <c r="E35" s="3">
         <v>-0.61699999999999999</v>
@@ -1596,13 +1653,13 @@
         <v>15</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="C36" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D36" s="1" t="s">
-        <v>33</v>
+      <c r="D36" s="18">
+        <v>4756</v>
       </c>
       <c r="E36" s="3">
         <v>-0.50900000000000001</v>
@@ -1622,13 +1679,13 @@
         <v>15</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D37" s="1" t="s">
-        <v>33</v>
+      <c r="D37" s="18">
+        <v>4756</v>
       </c>
       <c r="E37" s="3">
         <v>-0.505</v>
@@ -1651,10 +1708,10 @@
         <v>8</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="D38" s="1" t="s">
-        <v>33</v>
+        <v>38</v>
+      </c>
+      <c r="D38" s="18">
+        <v>4756</v>
       </c>
       <c r="E38" s="3">
         <v>-0.375</v>
@@ -1677,10 +1734,10 @@
         <v>9</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="D39" s="1" t="s">
-        <v>33</v>
+        <v>38</v>
+      </c>
+      <c r="D39" s="18">
+        <v>4756</v>
       </c>
       <c r="E39" s="3">
         <v>-0.437</v>
@@ -1700,13 +1757,13 @@
         <v>15</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="D40" s="1" t="s">
-        <v>33</v>
+        <v>38</v>
+      </c>
+      <c r="D40" s="18">
+        <v>4756</v>
       </c>
       <c r="E40" s="3">
         <v>-0.438</v>
@@ -1726,13 +1783,13 @@
         <v>15</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D41" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
+      </c>
+      <c r="D41" s="18">
+        <v>4756</v>
       </c>
       <c r="E41" s="3">
         <v>-0.13800000000000001</v>
@@ -1748,44 +1805,47 @@
       </c>
     </row>
     <row r="42" spans="1:8" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A42" s="1" t="s">
+      <c r="A42" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="B42" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="C42" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D42" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E42" s="3">
+      <c r="B42" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="C42" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="D42" s="19">
+        <v>4756</v>
+      </c>
+      <c r="E42" s="14">
         <v>-0.14000000000000001</v>
       </c>
-      <c r="F42" s="3">
+      <c r="F42" s="14">
         <v>-0.23499999999999999</v>
       </c>
-      <c r="G42" s="3">
+      <c r="G42" s="14">
         <v>-4.4999999999999998E-2</v>
       </c>
-      <c r="H42" s="1">
+      <c r="H42" s="13">
         <v>8.9999999999999993E-3</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="76" orientation="landscape" horizontalDpi="4294967293" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36E6E3BF-169C-40AF-9ABE-1F1C5BD901FE}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:AL108"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="F37" sqref="F37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.25" x14ac:dyDescent="0.3"/>
@@ -1793,14 +1853,16 @@
     <col min="1" max="1" width="31.375" customWidth="1"/>
     <col min="2" max="2" width="30.5" customWidth="1"/>
     <col min="3" max="3" width="6.625" style="10" customWidth="1"/>
-    <col min="4" max="4" width="9.375" bestFit="1" customWidth="1"/>
-    <col min="5" max="7" width="9.125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.75" customWidth="1"/>
+    <col min="5" max="5" width="13.625" customWidth="1"/>
+    <col min="6" max="6" width="13.375" customWidth="1"/>
+    <col min="7" max="7" width="9.125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="9"/>
@@ -1810,35 +1872,35 @@
       <c r="G1" s="2"/>
     </row>
     <row r="2" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F2" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="G2" s="12" t="s">
         <v>1</v>
       </c>
       <c r="H2" s="1"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="C3" s="10">
         <v>905</v>
@@ -1859,7 +1921,7 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>19</v>
@@ -1883,7 +1945,7 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>21</v>
@@ -1907,10 +1969,10 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="C6" s="10">
         <v>2881</v>
@@ -1931,10 +1993,10 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="C7" s="10">
         <v>2682</v>
@@ -1955,7 +2017,7 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>22</v>
@@ -1979,7 +2041,7 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>24</v>
@@ -2003,10 +2065,10 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="C10" s="10">
         <v>3219</v>
@@ -2027,10 +2089,10 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="C11" s="10">
         <v>2084</v>
@@ -2051,10 +2113,10 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="C12" s="10">
         <v>3248</v>
@@ -2075,10 +2137,10 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="C13" s="10">
         <v>3321</v>
@@ -2099,10 +2161,10 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="C14" s="10">
         <v>492</v>
@@ -2123,7 +2185,7 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>19</v>
@@ -2147,7 +2209,7 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>21</v>
@@ -2171,10 +2233,10 @@
     </row>
     <row r="17" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="C17" s="10">
         <v>2616</v>
@@ -2195,10 +2257,10 @@
     </row>
     <row r="18" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="C18" s="10">
         <v>1923</v>
@@ -2219,7 +2281,7 @@
     </row>
     <row r="19" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>22</v>
@@ -2243,7 +2305,7 @@
     </row>
     <row r="20" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>24</v>
@@ -2296,10 +2358,10 @@
     </row>
     <row r="21" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="C21" s="10">
         <v>3119</v>
@@ -2349,10 +2411,10 @@
     </row>
     <row r="22" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="C22" s="10">
         <v>2324</v>
@@ -2402,10 +2464,10 @@
     </row>
     <row r="23" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="C23" s="10">
         <v>3262</v>
@@ -2455,10 +2517,10 @@
     </row>
     <row r="24" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="C24" s="10">
         <v>3320</v>
@@ -2508,10 +2570,10 @@
     </row>
     <row r="25" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="C25" s="10">
         <v>356</v>
@@ -2561,7 +2623,7 @@
     </row>
     <row r="26" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>19</v>
@@ -2614,7 +2676,7 @@
     </row>
     <row r="27" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>21</v>
@@ -2667,10 +2729,10 @@
     </row>
     <row r="28" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="C28" s="10">
         <v>510</v>
@@ -2720,10 +2782,10 @@
     </row>
     <row r="29" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="C29" s="10">
         <v>490</v>
@@ -2773,7 +2835,7 @@
     </row>
     <row r="30" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>22</v>
@@ -2826,7 +2888,7 @@
     </row>
     <row r="31" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>24</v>
@@ -2879,10 +2941,10 @@
     </row>
     <row r="32" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="C32" s="10">
         <v>523</v>
@@ -2932,10 +2994,10 @@
     </row>
     <row r="33" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="C33" s="10">
         <v>496</v>
@@ -2985,10 +3047,10 @@
     </row>
     <row r="34" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="C34" s="10">
         <v>534</v>
@@ -3036,25 +3098,25 @@
       <c r="AL34" s="1"/>
     </row>
     <row r="35" spans="1:38" x14ac:dyDescent="0.3">
-      <c r="A35" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="B35" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="C35" s="10">
+      <c r="A35" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="B35" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="C35" s="15">
         <v>537</v>
       </c>
-      <c r="D35" s="4">
+      <c r="D35" s="16">
         <v>0.45637877737659899</v>
       </c>
-      <c r="E35" s="4">
+      <c r="E35" s="16">
         <v>0.38838599790253298</v>
       </c>
-      <c r="F35" s="4">
+      <c r="F35" s="16">
         <v>0.52232358635089404</v>
       </c>
-      <c r="G35" s="1" t="s">
+      <c r="G35" s="13" t="s">
         <v>4</v>
       </c>
       <c r="H35" s="6"/>
@@ -5514,27 +5576,33 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="91" orientation="landscape" horizontalDpi="4294967293" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34C0762C-5F45-4DA4-B2B6-A78222BA4808}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:H138"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A125" workbookViewId="0">
-      <selection activeCell="S144" sqref="S144"/>
+    <sheetView tabSelected="1" topLeftCell="B65" workbookViewId="0">
+      <selection activeCell="E76" sqref="E76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="34.75" customWidth="1"/>
-    <col min="3" max="3" width="21.75" customWidth="1"/>
+    <col min="1" max="1" width="30.375" customWidth="1"/>
+    <col min="3" max="3" width="23.25" customWidth="1"/>
+    <col min="5" max="5" width="12.875" customWidth="1"/>
+    <col min="6" max="6" width="13.375" customWidth="1"/>
+    <col min="7" max="7" width="13.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -5545,34 +5613,34 @@
       <c r="H1" s="1"/>
     </row>
     <row r="2" spans="1:8" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F2" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="G2" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="H2" s="12" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
       <c r="B3" s="1">
         <v>20</v>
@@ -5598,7 +5666,7 @@
     </row>
     <row r="4" spans="1:8" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="B4" s="1">
         <v>25</v>
@@ -5624,7 +5692,7 @@
     </row>
     <row r="5" spans="1:8" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="B5" s="1">
         <v>30</v>
@@ -5650,7 +5718,7 @@
     </row>
     <row r="6" spans="1:8" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="B6" s="1">
         <v>35</v>
@@ -5676,7 +5744,7 @@
     </row>
     <row r="7" spans="1:8" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="B7" s="1">
         <v>40</v>
@@ -5702,7 +5770,7 @@
     </row>
     <row r="8" spans="1:8" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="B8" s="1">
         <v>45</v>
@@ -5728,7 +5796,7 @@
     </row>
     <row r="9" spans="1:8" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="B9" s="1">
         <v>50</v>
@@ -5754,7 +5822,7 @@
     </row>
     <row r="10" spans="1:8" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="B10" s="1">
         <v>55</v>
@@ -5780,7 +5848,7 @@
     </row>
     <row r="11" spans="1:8" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="B11" s="1">
         <v>60</v>
@@ -5806,7 +5874,7 @@
     </row>
     <row r="12" spans="1:8" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="B12" s="1">
         <v>65</v>
@@ -5832,7 +5900,7 @@
     </row>
     <row r="13" spans="1:8" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="B13" s="1">
         <v>70</v>
@@ -5858,7 +5926,7 @@
     </row>
     <row r="14" spans="1:8" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="B14" s="1">
         <v>75</v>
@@ -5884,7 +5952,7 @@
     </row>
     <row r="15" spans="1:8" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="B15" s="1">
         <v>80</v>
@@ -5910,7 +5978,7 @@
     </row>
     <row r="16" spans="1:8" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="B16" s="1">
         <v>85</v>
@@ -5936,7 +6004,7 @@
     </row>
     <row r="17" spans="1:8" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="B17" s="1">
         <v>90</v>
@@ -5962,7 +6030,7 @@
     </row>
     <row r="18" spans="1:8" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="B18" s="1">
         <v>95</v>
@@ -5988,7 +6056,7 @@
     </row>
     <row r="19" spans="1:8" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="B19" s="1">
         <v>100</v>
@@ -6014,7 +6082,7 @@
     </row>
     <row r="20" spans="1:8" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="B20" s="1">
         <v>105</v>
@@ -6040,7 +6108,7 @@
     </row>
     <row r="21" spans="1:8" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="B21" s="1">
         <v>110</v>
@@ -6066,7 +6134,7 @@
     </row>
     <row r="22" spans="1:8" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="B22" s="1">
         <v>115</v>
@@ -6092,7 +6160,7 @@
     </row>
     <row r="23" spans="1:8" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="B23" s="1">
         <v>120</v>
@@ -6118,7 +6186,7 @@
     </row>
     <row r="24" spans="1:8" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="B24" s="1">
         <v>20</v>
@@ -6144,7 +6212,7 @@
     </row>
     <row r="25" spans="1:8" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="B25" s="1">
         <v>25</v>
@@ -6170,7 +6238,7 @@
     </row>
     <row r="26" spans="1:8" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="B26" s="1">
         <v>30</v>
@@ -6196,7 +6264,7 @@
     </row>
     <row r="27" spans="1:8" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="B27" s="1">
         <v>35</v>
@@ -6222,7 +6290,7 @@
     </row>
     <row r="28" spans="1:8" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="B28" s="1">
         <v>40</v>
@@ -6248,7 +6316,7 @@
     </row>
     <row r="29" spans="1:8" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="B29" s="1">
         <v>45</v>
@@ -6274,7 +6342,7 @@
     </row>
     <row r="30" spans="1:8" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="B30" s="1">
         <v>50</v>
@@ -6300,7 +6368,7 @@
     </row>
     <row r="31" spans="1:8" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="B31" s="1">
         <v>55</v>
@@ -6326,7 +6394,7 @@
     </row>
     <row r="32" spans="1:8" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="B32" s="1">
         <v>60</v>
@@ -6352,7 +6420,7 @@
     </row>
     <row r="33" spans="1:8" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="B33" s="1">
         <v>65</v>
@@ -6378,7 +6446,7 @@
     </row>
     <row r="34" spans="1:8" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="B34" s="1">
         <v>70</v>
@@ -6404,7 +6472,7 @@
     </row>
     <row r="35" spans="1:8" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="B35" s="1">
         <v>75</v>
@@ -6430,7 +6498,7 @@
     </row>
     <row r="36" spans="1:8" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="B36" s="1">
         <v>80</v>
@@ -6456,7 +6524,7 @@
     </row>
     <row r="37" spans="1:8" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="B37" s="1">
         <v>85</v>
@@ -6482,7 +6550,7 @@
     </row>
     <row r="38" spans="1:8" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="B38" s="1">
         <v>90</v>
@@ -6508,7 +6576,7 @@
     </row>
     <row r="39" spans="1:8" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="B39" s="1">
         <v>95</v>
@@ -6534,7 +6602,7 @@
     </row>
     <row r="40" spans="1:8" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="B40" s="1">
         <v>100</v>
@@ -6560,7 +6628,7 @@
     </row>
     <row r="41" spans="1:8" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="B41" s="1">
         <v>105</v>
@@ -6586,7 +6654,7 @@
     </row>
     <row r="42" spans="1:8" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="B42" s="1">
         <v>110</v>
@@ -6612,7 +6680,7 @@
     </row>
     <row r="43" spans="1:8" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="B43" s="1">
         <v>115</v>
@@ -6638,7 +6706,7 @@
     </row>
     <row r="44" spans="1:8" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="B44" s="1">
         <v>120</v>
@@ -6664,7 +6732,7 @@
     </row>
     <row r="45" spans="1:8" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="B45" s="1">
         <v>20</v>
@@ -6690,7 +6758,7 @@
     </row>
     <row r="46" spans="1:8" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="B46" s="1">
         <v>25</v>
@@ -6716,7 +6784,7 @@
     </row>
     <row r="47" spans="1:8" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="B47" s="1">
         <v>30</v>
@@ -6742,7 +6810,7 @@
     </row>
     <row r="48" spans="1:8" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="B48" s="1">
         <v>35</v>
@@ -6768,7 +6836,7 @@
     </row>
     <row r="49" spans="1:8" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A49" s="1" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="B49" s="1">
         <v>40</v>
@@ -6794,7 +6862,7 @@
     </row>
     <row r="50" spans="1:8" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A50" s="1" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="B50" s="1">
         <v>45</v>
@@ -6820,7 +6888,7 @@
     </row>
     <row r="51" spans="1:8" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A51" s="1" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="B51" s="1">
         <v>50</v>
@@ -6846,7 +6914,7 @@
     </row>
     <row r="52" spans="1:8" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A52" s="1" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="B52" s="1">
         <v>55</v>
@@ -6872,7 +6940,7 @@
     </row>
     <row r="53" spans="1:8" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A53" s="1" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="B53" s="1">
         <v>60</v>
@@ -6898,7 +6966,7 @@
     </row>
     <row r="54" spans="1:8" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A54" s="1" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="B54" s="1">
         <v>65</v>
@@ -6924,7 +6992,7 @@
     </row>
     <row r="55" spans="1:8" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A55" s="1" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="B55" s="1">
         <v>70</v>
@@ -6950,7 +7018,7 @@
     </row>
     <row r="56" spans="1:8" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A56" s="1" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="B56" s="1">
         <v>75</v>
@@ -6976,7 +7044,7 @@
     </row>
     <row r="57" spans="1:8" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A57" s="1" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="B57" s="1">
         <v>80</v>
@@ -7002,7 +7070,7 @@
     </row>
     <row r="58" spans="1:8" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A58" s="1" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="B58" s="1">
         <v>20</v>
@@ -7028,7 +7096,7 @@
     </row>
     <row r="59" spans="1:8" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A59" s="1" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="B59" s="1">
         <v>25</v>
@@ -7054,7 +7122,7 @@
     </row>
     <row r="60" spans="1:8" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A60" s="1" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="B60" s="1">
         <v>30</v>
@@ -7080,7 +7148,7 @@
     </row>
     <row r="61" spans="1:8" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A61" s="1" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="B61" s="1">
         <v>35</v>
@@ -7106,7 +7174,7 @@
     </row>
     <row r="62" spans="1:8" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A62" s="1" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="B62" s="1">
         <v>40</v>
@@ -7132,7 +7200,7 @@
     </row>
     <row r="63" spans="1:8" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A63" s="1" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="B63" s="1">
         <v>45</v>
@@ -7158,7 +7226,7 @@
     </row>
     <row r="64" spans="1:8" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A64" s="1" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="B64" s="1">
         <v>50</v>
@@ -7184,7 +7252,7 @@
     </row>
     <row r="65" spans="1:8" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A65" s="1" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="B65" s="1">
         <v>55</v>
@@ -7210,7 +7278,7 @@
     </row>
     <row r="66" spans="1:8" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A66" s="1" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="B66" s="1">
         <v>60</v>
@@ -7236,7 +7304,7 @@
     </row>
     <row r="67" spans="1:8" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A67" s="1" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="B67" s="1">
         <v>65</v>
@@ -7262,7 +7330,7 @@
     </row>
     <row r="68" spans="1:8" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A68" s="1" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="B68" s="1">
         <v>70</v>
@@ -7288,7 +7356,7 @@
     </row>
     <row r="69" spans="1:8" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A69" s="1" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="B69" s="1">
         <v>75</v>
@@ -7314,7 +7382,7 @@
     </row>
     <row r="70" spans="1:8" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A70" s="1" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="B70" s="1">
         <v>80</v>
@@ -7340,25 +7408,25 @@
     </row>
     <row r="71" spans="1:8" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A71" s="1" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
       <c r="B71" s="1">
         <v>20</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="D71" s="5">
-        <v>3321</v>
+        <v>3320</v>
       </c>
       <c r="E71" s="3">
-        <v>0.50785590000000003</v>
+        <v>0.504</v>
       </c>
       <c r="F71" s="3">
-        <v>0.48217199999999999</v>
+        <v>0.47899999999999998</v>
       </c>
       <c r="G71" s="3">
-        <v>0.53266760000000002</v>
+        <v>0.52900000000000003</v>
       </c>
       <c r="H71" s="1" t="s">
         <v>4</v>
@@ -7366,25 +7434,25 @@
     </row>
     <row r="72" spans="1:8" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A72" s="1" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="B72" s="1">
         <v>25</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="D72" s="5">
-        <v>3321</v>
+        <v>3320</v>
       </c>
       <c r="E72" s="3">
-        <v>0.52828949999999997</v>
+        <v>0.51500000000000001</v>
       </c>
       <c r="F72" s="3">
-        <v>0.50332069999999995</v>
+        <v>0.49</v>
       </c>
       <c r="G72" s="3">
-        <v>0.55237689999999995</v>
+        <v>0.54</v>
       </c>
       <c r="H72" s="1" t="s">
         <v>4</v>
@@ -7392,25 +7460,25 @@
     </row>
     <row r="73" spans="1:8" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A73" s="1" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="B73" s="1">
         <v>30</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="D73" s="5">
         <v>3320</v>
       </c>
       <c r="E73" s="3">
-        <v>0.53438410000000003</v>
+        <v>0.52100000000000002</v>
       </c>
       <c r="F73" s="3">
-        <v>0.50963060000000004</v>
+        <v>0.496</v>
       </c>
       <c r="G73" s="3">
-        <v>0.55825380000000002</v>
+        <v>0.54500000000000004</v>
       </c>
       <c r="H73" s="1" t="s">
         <v>4</v>
@@ -7418,25 +7486,25 @@
     </row>
     <row r="74" spans="1:8" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A74" s="1" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="B74" s="1">
         <v>35</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="D74" s="5">
         <v>3321</v>
       </c>
       <c r="E74" s="3">
-        <v>0.53902119999999998</v>
+        <v>0.53300000000000003</v>
       </c>
       <c r="F74" s="3">
-        <v>0.51444000000000001</v>
+        <v>0.50800000000000001</v>
       </c>
       <c r="G74" s="3">
-        <v>0.56271740000000003</v>
+        <v>0.55600000000000005</v>
       </c>
       <c r="H74" s="1" t="s">
         <v>4</v>
@@ -7444,25 +7512,25 @@
     </row>
     <row r="75" spans="1:8" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A75" s="1" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="B75" s="1">
         <v>40</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="D75" s="5">
-        <v>3320</v>
+        <v>3321</v>
       </c>
       <c r="E75" s="3">
-        <v>0.54665779999999997</v>
+        <v>0.54200000000000004</v>
       </c>
       <c r="F75" s="3">
-        <v>0.52235370000000003</v>
+        <v>0.51700000000000002</v>
       </c>
       <c r="G75" s="3">
-        <v>0.57007450000000004</v>
+        <v>0.56499999999999995</v>
       </c>
       <c r="H75" s="1" t="s">
         <v>4</v>
@@ -7470,25 +7538,25 @@
     </row>
     <row r="76" spans="1:8" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A76" s="1" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="B76" s="1">
         <v>45</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="D76" s="5">
-        <v>3320</v>
+        <v>3321</v>
       </c>
       <c r="E76" s="3">
-        <v>0.55668099999999998</v>
+        <v>0.54700000000000004</v>
       </c>
       <c r="F76" s="3">
-        <v>0.5327518</v>
+        <v>0.52300000000000002</v>
       </c>
       <c r="G76" s="3">
-        <v>0.57972060000000003</v>
+        <v>0.56999999999999995</v>
       </c>
       <c r="H76" s="1" t="s">
         <v>4</v>
@@ -7496,25 +7564,25 @@
     </row>
     <row r="77" spans="1:8" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A77" s="1" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="B77" s="1">
         <v>50</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="D77" s="5">
         <v>3321</v>
       </c>
       <c r="E77" s="3">
-        <v>0.55896029999999997</v>
+        <v>0.55200000000000005</v>
       </c>
       <c r="F77" s="3">
-        <v>0.53512110000000002</v>
+        <v>0.52800000000000002</v>
       </c>
       <c r="G77" s="3">
-        <v>0.58191000000000004</v>
+        <v>0.57599999999999996</v>
       </c>
       <c r="H77" s="1" t="s">
         <v>4</v>
@@ -7522,25 +7590,25 @@
     </row>
     <row r="78" spans="1:8" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A78" s="1" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="B78" s="1">
         <v>55</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="D78" s="5">
         <v>3321</v>
       </c>
       <c r="E78" s="3">
-        <v>0.56640069999999998</v>
+        <v>0.55600000000000005</v>
       </c>
       <c r="F78" s="3">
-        <v>0.54284569999999999</v>
+        <v>0.53200000000000003</v>
       </c>
       <c r="G78" s="3">
-        <v>0.58906519999999996</v>
+        <v>0.57899999999999996</v>
       </c>
       <c r="H78" s="1" t="s">
         <v>4</v>
@@ -7548,25 +7616,25 @@
     </row>
     <row r="79" spans="1:8" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A79" s="1" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="B79" s="1">
         <v>60</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="D79" s="5">
         <v>3321</v>
       </c>
       <c r="E79" s="3">
-        <v>0.56935460000000004</v>
+        <v>0.56000000000000005</v>
       </c>
       <c r="F79" s="3">
-        <v>0.5459136</v>
+        <v>0.53600000000000003</v>
       </c>
       <c r="G79" s="3">
-        <v>0.59190489999999996</v>
+        <v>0.58299999999999996</v>
       </c>
       <c r="H79" s="1" t="s">
         <v>4</v>
@@ -7574,25 +7642,25 @@
     </row>
     <row r="80" spans="1:8" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A80" s="1" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="B80" s="1">
         <v>65</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="D80" s="5">
         <v>3321</v>
       </c>
       <c r="E80" s="3">
-        <v>0.57823040000000003</v>
+        <v>0.56799999999999995</v>
       </c>
       <c r="F80" s="3">
-        <v>0.55513559999999995</v>
+        <v>0.54500000000000004</v>
       </c>
       <c r="G80" s="3">
-        <v>0.60043429999999998</v>
+        <v>0.59099999999999997</v>
       </c>
       <c r="H80" s="1" t="s">
         <v>4</v>
@@ -7600,25 +7668,25 @@
     </row>
     <row r="81" spans="1:8" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A81" s="1" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="B81" s="1">
         <v>70</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="D81" s="5">
         <v>3321</v>
       </c>
       <c r="E81" s="3">
-        <v>0.57758310000000002</v>
+        <v>0.57599999999999996</v>
       </c>
       <c r="F81" s="3">
-        <v>0.55446280000000003</v>
+        <v>0.55200000000000005</v>
       </c>
       <c r="G81" s="3">
-        <v>0.59981240000000002</v>
+        <v>0.59799999999999998</v>
       </c>
       <c r="H81" s="1" t="s">
         <v>4</v>
@@ -7626,25 +7694,25 @@
     </row>
     <row r="82" spans="1:8" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A82" s="1" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="B82" s="1">
         <v>75</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="D82" s="5">
         <v>3321</v>
       </c>
       <c r="E82" s="3">
-        <v>0.57648980000000005</v>
+        <v>0.58299999999999996</v>
       </c>
       <c r="F82" s="3">
-        <v>0.55332669999999995</v>
+        <v>0.56100000000000005</v>
       </c>
       <c r="G82" s="3">
-        <v>0.59876209999999996</v>
+        <v>0.60499999999999998</v>
       </c>
       <c r="H82" s="1" t="s">
         <v>4</v>
@@ -7652,25 +7720,25 @@
     </row>
     <row r="83" spans="1:8" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A83" s="1" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="B83" s="1">
         <v>80</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="D83" s="5">
         <v>3321</v>
       </c>
       <c r="E83" s="3">
-        <v>0.57737059999999996</v>
+        <v>0.58599999999999997</v>
       </c>
       <c r="F83" s="3">
-        <v>0.55424200000000001</v>
+        <v>0.56299999999999994</v>
       </c>
       <c r="G83" s="3">
-        <v>0.59960829999999998</v>
+        <v>0.60699999999999998</v>
       </c>
       <c r="H83" s="1" t="s">
         <v>4</v>
@@ -7678,25 +7746,25 @@
     </row>
     <row r="84" spans="1:8" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A84" s="1" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="B84" s="1">
         <v>85</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="D84" s="5">
         <v>3321</v>
       </c>
       <c r="E84" s="3">
-        <v>0.57779179999999997</v>
+        <v>0.58599999999999997</v>
       </c>
       <c r="F84" s="3">
-        <v>0.55467979999999995</v>
+        <v>0.56299999999999994</v>
       </c>
       <c r="G84" s="3">
-        <v>0.60001300000000002</v>
+        <v>0.60799999999999998</v>
       </c>
       <c r="H84" s="1" t="s">
         <v>4</v>
@@ -7704,25 +7772,25 @@
     </row>
     <row r="85" spans="1:8" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A85" s="1" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="B85" s="1">
         <v>90</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="D85" s="5">
         <v>3321</v>
       </c>
       <c r="E85" s="3">
-        <v>0.5856249</v>
+        <v>0.58799999999999997</v>
       </c>
       <c r="F85" s="3">
-        <v>0.56282279999999996</v>
+        <v>0.56499999999999995</v>
       </c>
       <c r="G85" s="3">
-        <v>0.60753630000000003</v>
+        <v>0.61</v>
       </c>
       <c r="H85" s="1" t="s">
         <v>4</v>
@@ -7730,25 +7798,25 @@
     </row>
     <row r="86" spans="1:8" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A86" s="1" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="B86" s="1">
         <v>95</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="D86" s="5">
         <v>3321</v>
       </c>
       <c r="E86" s="3">
-        <v>0.58819069999999996</v>
+        <v>0.59099999999999997</v>
       </c>
       <c r="F86" s="3">
-        <v>0.56549119999999997</v>
+        <v>0.56799999999999995</v>
       </c>
       <c r="G86" s="3">
-        <v>0.60999990000000004</v>
+        <v>0.61199999999999999</v>
       </c>
       <c r="H86" s="1" t="s">
         <v>4</v>
@@ -7756,25 +7824,25 @@
     </row>
     <row r="87" spans="1:8" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A87" s="1" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="B87" s="1">
         <v>100</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="D87" s="5">
         <v>3321</v>
       </c>
       <c r="E87" s="3">
-        <v>0.5900166</v>
+        <v>0.59199999999999997</v>
       </c>
       <c r="F87" s="3">
-        <v>0.56739030000000001</v>
+        <v>0.56999999999999995</v>
       </c>
       <c r="G87" s="3">
-        <v>0.61175270000000004</v>
+        <v>0.61399999999999999</v>
       </c>
       <c r="H87" s="1" t="s">
         <v>4</v>
@@ -7782,25 +7850,25 @@
     </row>
     <row r="88" spans="1:8" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A88" s="1" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="B88" s="1">
         <v>105</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="D88" s="5">
         <v>3321</v>
       </c>
       <c r="E88" s="3">
-        <v>0.59402250000000001</v>
+        <v>0.59099999999999997</v>
       </c>
       <c r="F88" s="3">
-        <v>0.57155769999999995</v>
+        <v>0.56899999999999995</v>
       </c>
       <c r="G88" s="3">
-        <v>0.61559759999999997</v>
+        <v>0.61299999999999999</v>
       </c>
       <c r="H88" s="1" t="s">
         <v>4</v>
@@ -7808,25 +7876,25 @@
     </row>
     <row r="89" spans="1:8" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A89" s="1" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="B89" s="1">
         <v>110</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="D89" s="5">
         <v>3321</v>
       </c>
       <c r="E89" s="3">
-        <v>0.59422059999999999</v>
+        <v>0.59399999999999997</v>
       </c>
       <c r="F89" s="3">
-        <v>0.57176369999999999</v>
+        <v>0.57099999999999995</v>
       </c>
       <c r="G89" s="3">
-        <v>0.61578759999999999</v>
+        <v>0.61499999999999999</v>
       </c>
       <c r="H89" s="1" t="s">
         <v>4</v>
@@ -7834,25 +7902,25 @@
     </row>
     <row r="90" spans="1:8" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A90" s="1" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="B90" s="1">
         <v>115</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="D90" s="5">
         <v>3321</v>
       </c>
       <c r="E90" s="3">
-        <v>0.59334140000000002</v>
+        <v>0.59499999999999997</v>
       </c>
       <c r="F90" s="3">
-        <v>0.57084900000000005</v>
+        <v>0.57199999999999995</v>
       </c>
       <c r="G90" s="3">
-        <v>0.61494389999999999</v>
+        <v>0.61599999999999999</v>
       </c>
       <c r="H90" s="1" t="s">
         <v>4</v>
@@ -7860,25 +7928,25 @@
     </row>
     <row r="91" spans="1:8" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A91" s="1" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="B91" s="1">
         <v>120</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="D91" s="5">
         <v>3321</v>
       </c>
       <c r="E91" s="3">
-        <v>0.59352859999999996</v>
+        <v>0.59499999999999997</v>
       </c>
       <c r="F91" s="3">
-        <v>0.57104379999999999</v>
+        <v>0.57299999999999995</v>
       </c>
       <c r="G91" s="3">
-        <v>0.61512359999999999</v>
+        <v>0.61699999999999999</v>
       </c>
       <c r="H91" s="1" t="s">
         <v>4</v>
@@ -7886,25 +7954,25 @@
     </row>
     <row r="92" spans="1:8" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A92" s="1" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="B92" s="1">
         <v>20</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
       <c r="D92" s="5">
         <v>3321</v>
       </c>
       <c r="E92" s="3">
-        <v>0.59162749999999997</v>
+        <v>0.60199999999999998</v>
       </c>
       <c r="F92" s="3">
-        <v>0.56906590000000001</v>
+        <v>0.57999999999999996</v>
       </c>
       <c r="G92" s="3">
-        <v>0.61329889999999998</v>
+        <v>0.623</v>
       </c>
       <c r="H92" s="1" t="s">
         <v>4</v>
@@ -7912,25 +7980,25 @@
     </row>
     <row r="93" spans="1:8" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A93" s="1" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="B93" s="1">
         <v>25</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
       <c r="D93" s="5">
         <v>3321</v>
       </c>
       <c r="E93" s="3">
-        <v>0.60500580000000004</v>
+        <v>0.61899999999999999</v>
       </c>
       <c r="F93" s="3">
-        <v>0.5829898</v>
+        <v>0.59699999999999998</v>
       </c>
       <c r="G93" s="3">
-        <v>0.62613410000000003</v>
+        <v>0.63900000000000001</v>
       </c>
       <c r="H93" s="1" t="s">
         <v>4</v>
@@ -7938,25 +8006,25 @@
     </row>
     <row r="94" spans="1:8" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A94" s="1" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="B94" s="1">
         <v>30</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="D94" s="5">
         <v>3321</v>
       </c>
       <c r="E94" s="3">
-        <v>0.61176580000000003</v>
+        <v>0.623</v>
       </c>
       <c r="F94" s="3">
-        <v>0.59003030000000001</v>
+        <v>0.60199999999999998</v>
       </c>
       <c r="G94" s="3">
-        <v>0.63261520000000004</v>
+        <v>0.64400000000000002</v>
       </c>
       <c r="H94" s="1" t="s">
         <v>4</v>
@@ -7964,25 +8032,25 @@
     </row>
     <row r="95" spans="1:8" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A95" s="1" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="B95" s="1">
         <v>35</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="D95" s="5">
         <v>3321</v>
       </c>
       <c r="E95" s="3">
-        <v>0.61216139999999997</v>
+        <v>0.628</v>
       </c>
       <c r="F95" s="3">
-        <v>0.59044229999999998</v>
+        <v>0.60699999999999998</v>
       </c>
       <c r="G95" s="3">
-        <v>0.63299439999999996</v>
+        <v>0.64800000000000002</v>
       </c>
       <c r="H95" s="1" t="s">
         <v>4</v>
@@ -7990,25 +8058,25 @@
     </row>
     <row r="96" spans="1:8" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A96" s="1" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="B96" s="1">
         <v>40</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="D96" s="5">
         <v>3321</v>
       </c>
       <c r="E96" s="3">
-        <v>0.61628070000000001</v>
+        <v>0.63100000000000001</v>
       </c>
       <c r="F96" s="3">
-        <v>0.5947344</v>
+        <v>0.61</v>
       </c>
       <c r="G96" s="3">
-        <v>0.63694229999999996</v>
+        <v>0.65100000000000002</v>
       </c>
       <c r="H96" s="1" t="s">
         <v>4</v>
@@ -8016,25 +8084,25 @@
     </row>
     <row r="97" spans="1:8" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A97" s="1" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="B97" s="1">
         <v>45</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="D97" s="5">
         <v>3321</v>
       </c>
       <c r="E97" s="3">
-        <v>0.62454279999999995</v>
+        <v>0.63300000000000001</v>
       </c>
       <c r="F97" s="3">
-        <v>0.60334650000000001</v>
+        <v>0.61199999999999999</v>
       </c>
       <c r="G97" s="3">
-        <v>0.64485720000000002</v>
+        <v>0.65300000000000002</v>
       </c>
       <c r="H97" s="1" t="s">
         <v>4</v>
@@ -8042,25 +8110,25 @@
     </row>
     <row r="98" spans="1:8" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A98" s="1" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="B98" s="1">
         <v>50</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="D98" s="5">
         <v>3321</v>
       </c>
       <c r="E98" s="3">
-        <v>0.62680179999999996</v>
+        <v>0.63200000000000001</v>
       </c>
       <c r="F98" s="3">
-        <v>0.60570210000000002</v>
+        <v>0.61199999999999999</v>
       </c>
       <c r="G98" s="3">
-        <v>0.6470205</v>
+        <v>0.65200000000000002</v>
       </c>
       <c r="H98" s="1" t="s">
         <v>4</v>
@@ -8068,25 +8136,25 @@
     </row>
     <row r="99" spans="1:8" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A99" s="1" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="B99" s="1">
         <v>55</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="D99" s="5">
         <v>3321</v>
       </c>
       <c r="E99" s="3">
-        <v>0.62616360000000004</v>
+        <v>0.63</v>
       </c>
       <c r="F99" s="3">
-        <v>0.60503660000000004</v>
+        <v>0.60899999999999999</v>
       </c>
       <c r="G99" s="3">
-        <v>0.64640949999999997</v>
+        <v>0.65</v>
       </c>
       <c r="H99" s="1" t="s">
         <v>4</v>
@@ -8094,25 +8162,25 @@
     </row>
     <row r="100" spans="1:8" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A100" s="1" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="B100" s="1">
         <v>60</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="D100" s="5">
         <v>3321</v>
       </c>
       <c r="E100" s="3">
-        <v>0.62507040000000003</v>
+        <v>0.63300000000000001</v>
       </c>
       <c r="F100" s="3">
-        <v>0.60389669999999995</v>
+        <v>0.61299999999999999</v>
       </c>
       <c r="G100" s="3">
-        <v>0.64536249999999995</v>
+        <v>0.65300000000000002</v>
       </c>
       <c r="H100" s="1" t="s">
         <v>4</v>
@@ -8120,25 +8188,25 @@
     </row>
     <row r="101" spans="1:8" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A101" s="1" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="B101" s="1">
         <v>65</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="D101" s="5">
         <v>3321</v>
       </c>
       <c r="E101" s="3">
-        <v>0.63346959999999997</v>
+        <v>0.63800000000000001</v>
       </c>
       <c r="F101" s="3">
-        <v>0.61265720000000001</v>
+        <v>0.61799999999999999</v>
       </c>
       <c r="G101" s="3">
-        <v>0.65340410000000004</v>
+        <v>0.65800000000000003</v>
       </c>
       <c r="H101" s="1" t="s">
         <v>4</v>
@@ -8146,25 +8214,25 @@
     </row>
     <row r="102" spans="1:8" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A102" s="1" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="B102" s="1">
         <v>70</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="D102" s="5">
         <v>3321</v>
       </c>
       <c r="E102" s="3">
-        <v>0.63313850000000005</v>
+        <v>0.63700000000000001</v>
       </c>
       <c r="F102" s="3">
-        <v>0.61231179999999996</v>
+        <v>0.61599999999999999</v>
       </c>
       <c r="G102" s="3">
-        <v>0.65308719999999998</v>
+        <v>0.65600000000000003</v>
       </c>
       <c r="H102" s="1" t="s">
         <v>4</v>
@@ -8172,25 +8240,25 @@
     </row>
     <row r="103" spans="1:8" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A103" s="1" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="B103" s="1">
         <v>75</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="D103" s="5">
         <v>3321</v>
       </c>
       <c r="E103" s="3">
-        <v>0.63032909999999998</v>
+        <v>0.64100000000000001</v>
       </c>
       <c r="F103" s="3">
-        <v>0.60938099999999995</v>
+        <v>0.621</v>
       </c>
       <c r="G103" s="3">
-        <v>0.65039780000000003</v>
+        <v>0.66100000000000003</v>
       </c>
       <c r="H103" s="1" t="s">
         <v>4</v>
@@ -8198,25 +8266,25 @@
     </row>
     <row r="104" spans="1:8" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A104" s="1" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="B104" s="1">
         <v>80</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="D104" s="5">
         <v>3321</v>
       </c>
       <c r="E104" s="3">
-        <v>0.63161690000000004</v>
+        <v>0.63900000000000001</v>
       </c>
       <c r="F104" s="3">
-        <v>0.61072439999999995</v>
+        <v>0.61799999999999999</v>
       </c>
       <c r="G104" s="3">
-        <v>0.65163070000000001</v>
+        <v>0.65900000000000003</v>
       </c>
       <c r="H104" s="1" t="s">
         <v>4</v>
@@ -8224,25 +8292,25 @@
     </row>
     <row r="105" spans="1:8" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A105" s="1" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="B105" s="1">
         <v>85</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="D105" s="5">
         <v>3321</v>
       </c>
       <c r="E105" s="3">
-        <v>0.63232999999999995</v>
+        <v>0.64</v>
       </c>
       <c r="F105" s="3">
-        <v>0.61146829999999996</v>
+        <v>0.61899999999999999</v>
       </c>
       <c r="G105" s="3">
-        <v>0.65231329999999998</v>
+        <v>0.66</v>
       </c>
       <c r="H105" s="1" t="s">
         <v>4</v>
@@ -8250,25 +8318,25 @@
     </row>
     <row r="106" spans="1:8" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A106" s="1" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="B106" s="1">
         <v>90</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="D106" s="5">
         <v>3321</v>
       </c>
       <c r="E106" s="3">
-        <v>0.63291459999999999</v>
+        <v>0.64200000000000002</v>
       </c>
       <c r="F106" s="3">
-        <v>0.61207809999999996</v>
+        <v>0.622</v>
       </c>
       <c r="G106" s="3">
-        <v>0.65287289999999998</v>
+        <v>0.66200000000000003</v>
       </c>
       <c r="H106" s="1" t="s">
         <v>4</v>
@@ -8276,25 +8344,25 @@
     </row>
     <row r="107" spans="1:8" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A107" s="1" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="B107" s="1">
         <v>95</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="D107" s="5">
         <v>3321</v>
       </c>
       <c r="E107" s="3">
-        <v>0.63360490000000003</v>
+        <v>0.64400000000000002</v>
       </c>
       <c r="F107" s="3">
-        <v>0.61279830000000002</v>
+        <v>0.624</v>
       </c>
       <c r="G107" s="3">
-        <v>0.65353360000000005</v>
+        <v>0.66400000000000003</v>
       </c>
       <c r="H107" s="1" t="s">
         <v>4</v>
@@ -8302,25 +8370,25 @@
     </row>
     <row r="108" spans="1:8" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A108" s="1" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="B108" s="1">
         <v>100</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="D108" s="5">
         <v>3321</v>
       </c>
       <c r="E108" s="3">
-        <v>0.63458150000000002</v>
+        <v>0.64600000000000002</v>
       </c>
       <c r="F108" s="3">
-        <v>0.61381719999999995</v>
+        <v>0.625</v>
       </c>
       <c r="G108" s="3">
-        <v>0.6544683</v>
+        <v>0.66500000000000004</v>
       </c>
       <c r="H108" s="1" t="s">
         <v>4</v>
@@ -8328,25 +8396,25 @@
     </row>
     <row r="109" spans="1:8" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A109" s="1" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="B109" s="1">
         <v>105</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="D109" s="5">
         <v>3321</v>
       </c>
       <c r="E109" s="3">
-        <v>0.63185910000000001</v>
+        <v>0.64700000000000002</v>
       </c>
       <c r="F109" s="3">
-        <v>0.61097699999999999</v>
+        <v>0.627</v>
       </c>
       <c r="G109" s="3">
-        <v>0.65186250000000001</v>
+        <v>0.66600000000000004</v>
       </c>
       <c r="H109" s="1" t="s">
         <v>4</v>
@@ -8354,25 +8422,25 @@
     </row>
     <row r="110" spans="1:8" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A110" s="1" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="B110" s="1">
         <v>110</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="D110" s="5">
         <v>3321</v>
       </c>
       <c r="E110" s="3">
-        <v>0.63265229999999995</v>
+        <v>0.64800000000000002</v>
       </c>
       <c r="F110" s="3">
-        <v>0.61180449999999997</v>
+        <v>0.628</v>
       </c>
       <c r="G110" s="3">
-        <v>0.65262180000000003</v>
+        <v>0.66700000000000004</v>
       </c>
       <c r="H110" s="1" t="s">
         <v>4</v>
@@ -8380,25 +8448,25 @@
     </row>
     <row r="111" spans="1:8" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A111" s="1" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="B111" s="1">
         <v>115</v>
       </c>
       <c r="C111" s="1" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="D111" s="5">
         <v>3321</v>
       </c>
       <c r="E111" s="3">
-        <v>0.63296200000000002</v>
+        <v>0.64800000000000002</v>
       </c>
       <c r="F111" s="3">
-        <v>0.61212759999999999</v>
+        <v>0.628</v>
       </c>
       <c r="G111" s="3">
-        <v>0.65291829999999995</v>
+        <v>0.66800000000000004</v>
       </c>
       <c r="H111" s="1" t="s">
         <v>4</v>
@@ -8406,25 +8474,25 @@
     </row>
     <row r="112" spans="1:8" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A112" s="1" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="B112" s="1">
         <v>120</v>
       </c>
       <c r="C112" s="1" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="D112" s="5">
         <v>3321</v>
       </c>
       <c r="E112" s="3">
-        <v>0.63197709999999996</v>
+        <v>0.64900000000000002</v>
       </c>
       <c r="F112" s="3">
-        <v>0.61110010000000003</v>
+        <v>0.629</v>
       </c>
       <c r="G112" s="3">
-        <v>0.65197550000000004</v>
+        <v>0.66800000000000004</v>
       </c>
       <c r="H112" s="1" t="s">
         <v>4</v>
@@ -8432,25 +8500,25 @@
     </row>
     <row r="113" spans="1:8" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A113" s="1" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="B113" s="1">
         <v>20</v>
       </c>
       <c r="C113" s="1" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="D113" s="5">
         <v>3321</v>
       </c>
       <c r="E113" s="3">
-        <v>0.59588529999999995</v>
+        <v>0.629</v>
       </c>
       <c r="F113" s="3">
-        <v>0.57349600000000001</v>
+        <v>0.60799999999999998</v>
       </c>
       <c r="G113" s="3">
-        <v>0.61738510000000002</v>
+        <v>0.64900000000000002</v>
       </c>
       <c r="H113" s="1" t="s">
         <v>4</v>
@@ -8458,25 +8526,25 @@
     </row>
     <row r="114" spans="1:8" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A114" s="1" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="B114" s="1">
         <v>25</v>
       </c>
       <c r="C114" s="1" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="D114" s="5">
-        <v>3321</v>
+        <v>3320</v>
       </c>
       <c r="E114" s="3">
-        <v>0.61363840000000003</v>
+        <v>0.63300000000000001</v>
       </c>
       <c r="F114" s="3">
-        <v>0.59198119999999999</v>
+        <v>0.61199999999999999</v>
       </c>
       <c r="G114" s="3">
-        <v>0.63441009999999998</v>
+        <v>0.65300000000000002</v>
       </c>
       <c r="H114" s="1" t="s">
         <v>4</v>
@@ -8484,25 +8552,25 @@
     </row>
     <row r="115" spans="1:8" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A115" s="1" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="B115" s="1">
         <v>30</v>
       </c>
       <c r="C115" s="1" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="D115" s="5">
         <v>3321</v>
       </c>
       <c r="E115" s="3">
-        <v>0.6270964</v>
+        <v>0.63900000000000001</v>
       </c>
       <c r="F115" s="3">
-        <v>0.60600940000000003</v>
+        <v>0.61899999999999999</v>
       </c>
       <c r="G115" s="3">
-        <v>0.64730270000000001</v>
+        <v>0.65900000000000003</v>
       </c>
       <c r="H115" s="1" t="s">
         <v>4</v>
@@ -8510,25 +8578,25 @@
     </row>
     <row r="116" spans="1:8" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A116" s="1" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="B116" s="1">
         <v>35</v>
       </c>
       <c r="C116" s="1" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="D116" s="5">
         <v>3321</v>
       </c>
       <c r="E116" s="3">
-        <v>0.63749250000000002</v>
+        <v>0.64600000000000002</v>
       </c>
       <c r="F116" s="3">
-        <v>0.61685489999999998</v>
+        <v>0.626</v>
       </c>
       <c r="G116" s="3">
-        <v>0.65725409999999995</v>
+        <v>0.66500000000000004</v>
       </c>
       <c r="H116" s="1" t="s">
         <v>4</v>
@@ -8536,25 +8604,25 @@
     </row>
     <row r="117" spans="1:8" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A117" s="1" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="B117" s="1">
         <v>40</v>
       </c>
       <c r="C117" s="1" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="D117" s="5">
-        <v>3321</v>
+        <v>3320</v>
       </c>
       <c r="E117" s="3">
-        <v>0.64101560000000002</v>
+        <v>0.64500000000000002</v>
       </c>
       <c r="F117" s="3">
-        <v>0.62053210000000003</v>
+        <v>0.625</v>
       </c>
       <c r="G117" s="3">
-        <v>0.66062500000000002</v>
+        <v>0.66500000000000004</v>
       </c>
       <c r="H117" s="1" t="s">
         <v>4</v>
@@ -8562,25 +8630,25 @@
     </row>
     <row r="118" spans="1:8" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A118" s="1" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="B118" s="1">
         <v>45</v>
       </c>
       <c r="C118" s="1" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="D118" s="5">
         <v>3321</v>
       </c>
       <c r="E118" s="3">
-        <v>0.64527440000000003</v>
+        <v>0.65300000000000002</v>
       </c>
       <c r="F118" s="3">
-        <v>0.62497840000000005</v>
+        <v>0.63300000000000001</v>
       </c>
       <c r="G118" s="3">
-        <v>0.66469869999999998</v>
+        <v>0.67200000000000004</v>
       </c>
       <c r="H118" s="1" t="s">
         <v>4</v>
@@ -8588,25 +8656,25 @@
     </row>
     <row r="119" spans="1:8" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A119" s="1" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="B119" s="1">
         <v>50</v>
       </c>
       <c r="C119" s="1" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="D119" s="5">
         <v>3321</v>
       </c>
       <c r="E119" s="3">
-        <v>0.64929809999999999</v>
+        <v>0.65600000000000003</v>
       </c>
       <c r="F119" s="3">
-        <v>0.62918039999999997</v>
+        <v>0.63600000000000001</v>
       </c>
       <c r="G119" s="3">
-        <v>0.66854639999999999</v>
+        <v>0.67500000000000004</v>
       </c>
       <c r="H119" s="1" t="s">
         <v>4</v>
@@ -8614,25 +8682,25 @@
     </row>
     <row r="120" spans="1:8" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A120" s="1" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="B120" s="1">
         <v>55</v>
       </c>
       <c r="C120" s="1" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="D120" s="5">
         <v>3321</v>
       </c>
       <c r="E120" s="3">
-        <v>0.65785720000000003</v>
+        <v>0.66400000000000003</v>
       </c>
       <c r="F120" s="3">
-        <v>0.63812270000000004</v>
+        <v>0.64500000000000002</v>
       </c>
       <c r="G120" s="3">
-        <v>0.67672779999999999</v>
+        <v>0.68300000000000005</v>
       </c>
       <c r="H120" s="1" t="s">
         <v>4</v>
@@ -8640,25 +8708,25 @@
     </row>
     <row r="121" spans="1:8" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A121" s="1" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="B121" s="1">
         <v>60</v>
       </c>
       <c r="C121" s="1" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="D121" s="5">
         <v>3321</v>
       </c>
       <c r="E121" s="3">
-        <v>0.65609170000000006</v>
+        <v>0.66500000000000004</v>
       </c>
       <c r="F121" s="3">
-        <v>0.6362778</v>
+        <v>0.64600000000000002</v>
       </c>
       <c r="G121" s="3">
-        <v>0.67504070000000005</v>
+        <v>0.68400000000000005</v>
       </c>
       <c r="H121" s="1" t="s">
         <v>4</v>
@@ -8666,25 +8734,25 @@
     </row>
     <row r="122" spans="1:8" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A122" s="1" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="B122" s="1">
         <v>65</v>
       </c>
       <c r="C122" s="1" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="D122" s="5">
         <v>3321</v>
       </c>
       <c r="E122" s="3">
-        <v>0.65629899999999997</v>
+        <v>0.66600000000000004</v>
       </c>
       <c r="F122" s="3">
-        <v>0.63649440000000002</v>
+        <v>0.64700000000000002</v>
       </c>
       <c r="G122" s="3">
-        <v>0.67523880000000003</v>
+        <v>0.68500000000000005</v>
       </c>
       <c r="H122" s="1" t="s">
         <v>4</v>
@@ -8692,25 +8760,25 @@
     </row>
     <row r="123" spans="1:8" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A123" s="1" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="B123" s="1">
         <v>70</v>
       </c>
       <c r="C123" s="1" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="D123" s="5">
         <v>3321</v>
       </c>
       <c r="E123" s="3">
-        <v>0.66111450000000005</v>
+        <v>0.66600000000000004</v>
       </c>
       <c r="F123" s="3">
-        <v>0.64152730000000002</v>
+        <v>0.64700000000000002</v>
       </c>
       <c r="G123" s="3">
-        <v>0.67984009999999995</v>
+        <v>0.68400000000000005</v>
       </c>
       <c r="H123" s="1" t="s">
         <v>4</v>
@@ -8718,25 +8786,25 @@
     </row>
     <row r="124" spans="1:8" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A124" s="1" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="B124" s="1">
         <v>75</v>
       </c>
       <c r="C124" s="1" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="D124" s="5">
         <v>3321</v>
       </c>
       <c r="E124" s="3">
-        <v>0.66426529999999995</v>
+        <v>0.66900000000000004</v>
       </c>
       <c r="F124" s="3">
-        <v>0.64482130000000004</v>
+        <v>0.64900000000000002</v>
       </c>
       <c r="G124" s="3">
-        <v>0.68285010000000002</v>
+        <v>0.68700000000000006</v>
       </c>
       <c r="H124" s="1" t="s">
         <v>4</v>
@@ -8744,25 +8812,25 @@
     </row>
     <row r="125" spans="1:8" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A125" s="1" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="B125" s="1">
         <v>80</v>
       </c>
       <c r="C125" s="1" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="D125" s="5">
         <v>3321</v>
       </c>
       <c r="E125" s="3">
-        <v>0.66924209999999995</v>
+        <v>0.67100000000000004</v>
       </c>
       <c r="F125" s="3">
-        <v>0.65002570000000004</v>
+        <v>0.65100000000000002</v>
       </c>
       <c r="G125" s="3">
-        <v>0.68760310000000002</v>
+        <v>0.68899999999999995</v>
       </c>
       <c r="H125" s="1" t="s">
         <v>4</v>
@@ -8770,25 +8838,25 @@
     </row>
     <row r="126" spans="1:8" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A126" s="1" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="B126" s="1">
         <v>20</v>
       </c>
       <c r="C126" s="1" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="D126" s="5">
         <v>3321</v>
       </c>
       <c r="E126" s="3">
-        <v>0.71290379999999998</v>
+        <v>0.71699999999999997</v>
       </c>
       <c r="F126" s="3">
-        <v>0.69576179999999999</v>
+        <v>0.7</v>
       </c>
       <c r="G126" s="3">
-        <v>0.7292343</v>
+        <v>0.73299999999999998</v>
       </c>
       <c r="H126" s="1" t="s">
         <v>4</v>
@@ -8796,25 +8864,25 @@
     </row>
     <row r="127" spans="1:8" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A127" s="1" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="B127" s="1">
         <v>25</v>
       </c>
       <c r="C127" s="1" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="D127" s="5">
         <v>3321</v>
       </c>
       <c r="E127" s="3">
-        <v>0.71859479999999998</v>
+        <v>0.72</v>
       </c>
       <c r="F127" s="3">
-        <v>0.70173339999999995</v>
+        <v>0.70299999999999996</v>
       </c>
       <c r="G127" s="3">
-        <v>0.73465170000000002</v>
+        <v>0.73599999999999999</v>
       </c>
       <c r="H127" s="1" t="s">
         <v>4</v>
@@ -8822,25 +8890,25 @@
     </row>
     <row r="128" spans="1:8" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A128" s="1" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="B128" s="1">
         <v>30</v>
       </c>
       <c r="C128" s="1" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="D128" s="5">
         <v>3321</v>
       </c>
       <c r="E128" s="3">
-        <v>0.72842090000000004</v>
+        <v>0.72399999999999998</v>
       </c>
       <c r="F128" s="3">
-        <v>0.71204959999999995</v>
+        <v>0.70799999999999996</v>
       </c>
       <c r="G128" s="3">
-        <v>0.74400060000000001</v>
+        <v>0.74</v>
       </c>
       <c r="H128" s="1" t="s">
         <v>4</v>
@@ -8848,25 +8916,25 @@
     </row>
     <row r="129" spans="1:8" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A129" s="1" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="B129" s="1">
         <v>35</v>
       </c>
       <c r="C129" s="1" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="D129" s="5">
         <v>3321</v>
       </c>
       <c r="E129" s="3">
-        <v>0.73726769999999997</v>
+        <v>0.73</v>
       </c>
       <c r="F129" s="3">
-        <v>0.72134379999999998</v>
+        <v>0.71299999999999997</v>
       </c>
       <c r="G129" s="3">
-        <v>0.75241259999999999</v>
+        <v>0.745</v>
       </c>
       <c r="H129" s="1" t="s">
         <v>4</v>
@@ -8874,25 +8942,25 @@
     </row>
     <row r="130" spans="1:8" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A130" s="1" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="B130" s="1">
         <v>40</v>
       </c>
       <c r="C130" s="1" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="D130" s="5">
         <v>3321</v>
       </c>
       <c r="E130" s="3">
-        <v>0.73670919999999995</v>
+        <v>0.73099999999999998</v>
       </c>
       <c r="F130" s="3">
-        <v>0.72075679999999998</v>
+        <v>0.71499999999999997</v>
       </c>
       <c r="G130" s="3">
-        <v>0.75188169999999999</v>
+        <v>0.746</v>
       </c>
       <c r="H130" s="1" t="s">
         <v>4</v>
@@ -8900,25 +8968,25 @@
     </row>
     <row r="131" spans="1:8" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A131" s="1" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="B131" s="1">
         <v>45</v>
       </c>
       <c r="C131" s="1" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="D131" s="5">
         <v>3321</v>
       </c>
       <c r="E131" s="3">
-        <v>0.73784280000000002</v>
+        <v>0.73299999999999998</v>
       </c>
       <c r="F131" s="3">
-        <v>0.72194809999999998</v>
+        <v>0.71699999999999997</v>
       </c>
       <c r="G131" s="3">
-        <v>0.7529593</v>
+        <v>0.749</v>
       </c>
       <c r="H131" s="1" t="s">
         <v>4</v>
@@ -8926,25 +8994,25 @@
     </row>
     <row r="132" spans="1:8" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A132" s="1" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="B132" s="1">
         <v>50</v>
       </c>
       <c r="C132" s="1" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="D132" s="5">
         <v>3321</v>
       </c>
       <c r="E132" s="3">
-        <v>0.73803640000000004</v>
+        <v>0.73399999999999999</v>
       </c>
       <c r="F132" s="3">
-        <v>0.72215149999999995</v>
+        <v>0.71799999999999997</v>
       </c>
       <c r="G132" s="3">
-        <v>0.75314329999999996</v>
+        <v>0.75</v>
       </c>
       <c r="H132" s="1" t="s">
         <v>4</v>
@@ -8952,25 +9020,25 @@
     </row>
     <row r="133" spans="1:8" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A133" s="1" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="B133" s="1">
         <v>55</v>
       </c>
       <c r="C133" s="1" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="D133" s="5">
         <v>3321</v>
       </c>
       <c r="E133" s="3">
-        <v>0.73859200000000003</v>
+        <v>0.73699999999999999</v>
       </c>
       <c r="F133" s="3">
-        <v>0.72273549999999998</v>
+        <v>0.72099999999999997</v>
       </c>
       <c r="G133" s="3">
-        <v>0.75367139999999999</v>
+        <v>0.752</v>
       </c>
       <c r="H133" s="1" t="s">
         <v>4</v>
@@ -8978,25 +9046,25 @@
     </row>
     <row r="134" spans="1:8" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A134" s="1" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="B134" s="1">
         <v>60</v>
       </c>
       <c r="C134" s="1" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="D134" s="5">
         <v>3321</v>
       </c>
       <c r="E134" s="3">
-        <v>0.73820260000000004</v>
+        <v>0.73799999999999999</v>
       </c>
       <c r="F134" s="3">
-        <v>0.72232620000000003</v>
+        <v>0.72199999999999998</v>
       </c>
       <c r="G134" s="3">
-        <v>0.75330129999999995</v>
+        <v>0.753</v>
       </c>
       <c r="H134" s="1" t="s">
         <v>4</v>
@@ -9004,25 +9072,25 @@
     </row>
     <row r="135" spans="1:8" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A135" s="1" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="B135" s="1">
         <v>65</v>
       </c>
       <c r="C135" s="1" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="D135" s="5">
         <v>3321</v>
       </c>
       <c r="E135" s="3">
-        <v>0.7403267</v>
+        <v>0.74099999999999999</v>
       </c>
       <c r="F135" s="3">
-        <v>0.7245587</v>
+        <v>0.72499999999999998</v>
       </c>
       <c r="G135" s="3">
-        <v>0.75532010000000005</v>
+        <v>0.75600000000000001</v>
       </c>
       <c r="H135" s="1" t="s">
         <v>4</v>
@@ -9030,25 +9098,25 @@
     </row>
     <row r="136" spans="1:8" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A136" s="1" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="B136" s="1">
         <v>70</v>
       </c>
       <c r="C136" s="1" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="D136" s="5">
         <v>3321</v>
       </c>
       <c r="E136" s="3">
-        <v>0.74327399999999999</v>
+        <v>0.74099999999999999</v>
       </c>
       <c r="F136" s="3">
-        <v>0.727657</v>
+        <v>0.72599999999999998</v>
       </c>
       <c r="G136" s="3">
-        <v>0.75812089999999999</v>
+        <v>0.75600000000000001</v>
       </c>
       <c r="H136" s="1" t="s">
         <v>4</v>
@@ -9056,58 +9124,59 @@
     </row>
     <row r="137" spans="1:8" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A137" s="1" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="B137" s="1">
         <v>75</v>
       </c>
       <c r="C137" s="1" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="D137" s="5">
         <v>3321</v>
       </c>
       <c r="E137" s="3">
-        <v>0.74276180000000003</v>
+        <v>0.74199999999999999</v>
       </c>
       <c r="F137" s="3">
-        <v>0.7271185</v>
+        <v>0.72599999999999998</v>
       </c>
       <c r="G137" s="3">
-        <v>0.75763420000000004</v>
+        <v>0.75600000000000001</v>
       </c>
       <c r="H137" s="1" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="138" spans="1:8" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A138" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="B138" s="1">
+      <c r="A138" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="B138" s="13">
         <v>80</v>
       </c>
-      <c r="C138" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="D138" s="5">
-        <v>3321</v>
-      </c>
-      <c r="E138" s="3">
-        <v>0.7442801</v>
-      </c>
-      <c r="F138" s="3">
-        <v>0.72871470000000005</v>
-      </c>
-      <c r="G138" s="3">
-        <v>0.7590768</v>
-      </c>
-      <c r="H138" s="1" t="s">
+      <c r="C138" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="D138" s="17">
+        <v>3321</v>
+      </c>
+      <c r="E138" s="14">
+        <v>0.74199999999999999</v>
+      </c>
+      <c r="F138" s="14">
+        <v>0.72599999999999998</v>
+      </c>
+      <c r="G138" s="14">
+        <v>0.75700000000000001</v>
+      </c>
+      <c r="H138" s="13" t="s">
         <v>4</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" scale="61" fitToHeight="0" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>